<commit_message>
Changed ROCff to ROCffmax
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295F99E2-EF97-4688-B93C-5DAD9E1F5035}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0546892F-9B0D-470E-A55B-579B474B8D74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
   <si>
     <t>Parameter</t>
   </si>
@@ -467,7 +466,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -747,19 +746,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -773,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -787,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -801,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -815,7 +814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -830,7 +829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -844,7 +843,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -858,12 +857,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="8">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -872,7 +871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -886,7 +885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="57" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -900,7 +899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -915,7 +914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -930,7 +929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -957,13 +956,13 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -977,7 +976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -991,7 +990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1030,7 +1029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1058,7 +1057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1100,7 +1099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -1114,7 +1113,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1142,7 +1141,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1185,14 +1184,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1236,7 +1235,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1264,7 +1263,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1278,7 +1277,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -1335,100 +1334,100 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
     </row>
   </sheetData>
@@ -1444,13 +1443,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1478,7 +1477,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1492,7 +1491,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Pimped out the design iteration function a little bit
Just ask me in case you are using the DesignIter function after this update
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0546892F-9B0D-470E-A55B-579B474B8D74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185A453F-20CB-4901-BE5C-BC600E872252}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
   <si>
     <t>Parameter</t>
   </si>
@@ -383,6 +383,39 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>MTOW</t>
+  </si>
+  <si>
+    <t>Maximum take-off weight</t>
+  </si>
+  <si>
+    <t>Nprops</t>
+  </si>
+  <si>
+    <t>Amount of VTOL propellers</t>
+  </si>
+  <si>
+    <t>Nblades</t>
+  </si>
+  <si>
+    <t>Amount of blades on the propeller</t>
+  </si>
+  <si>
+    <t>N/m2</t>
+  </si>
+  <si>
+    <t>Selected propeller disk loading</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Aspect ratio</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
 </sst>
 </file>
@@ -746,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -950,10 +983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A776EB1-CF70-4180-BDC5-FBCD4C7D05BD}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1123,7 @@
         <v>81</v>
       </c>
       <c r="B10" s="7">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1169,6 +1202,76 @@
       </c>
       <c r="D15" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16">
+        <v>3353.95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="7">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1300</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>